<commit_message>
updating statutory SAP and SMP files
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201718.xlsx
@@ -4,32 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="13" activeTab="15"/>
+    <workbookView activeTab="15" firstSheet="13" windowHeight="5400" windowWidth="15168" xWindow="384" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="2" r:id="rId1"/>
-    <sheet name="ResetData" sheetId="13" r:id="rId2"/>
-    <sheet name="CreateMaleEmployee" sheetId="14" r:id="rId3"/>
-    <sheet name="UpdateTaxCodeAndAnnualSalary" sheetId="15" r:id="rId4"/>
-    <sheet name="ProcessPayrolFor20FourWeeklySSP" sheetId="1" r:id="rId5"/>
-    <sheet name="ProcessPayrolFor24FourWeeklySSP" sheetId="3" r:id="rId6"/>
-    <sheet name="ProcessPayrolFor28FourWeeklySSP" sheetId="4" r:id="rId7"/>
-    <sheet name="CreateLeaveRequest" sheetId="9" r:id="rId8"/>
-    <sheet name="UpdateLeaveRecord" sheetId="10" r:id="rId9"/>
-    <sheet name="AverageWeeklyEarningsTestReport" sheetId="19" r:id="rId10"/>
-    <sheet name="ProcessPayrolFor32FourWeeklySSP" sheetId="6" r:id="rId11"/>
-    <sheet name="ProcessPayrolFor36FourWeeklySSP" sheetId="7" r:id="rId12"/>
-    <sheet name="CreateLeaveRequest2" sheetId="11" r:id="rId13"/>
-    <sheet name="UpdateLeaveRecord2" sheetId="12" r:id="rId14"/>
-    <sheet name="AverageWeeklyEarningsTestReprt2" sheetId="22" r:id="rId15"/>
-    <sheet name="ProcessPayrolFor40FourWeeklySSP" sheetId="8" r:id="rId16"/>
+    <sheet name="first" r:id="rId1" sheetId="2"/>
+    <sheet name="ResetData" r:id="rId2" sheetId="13"/>
+    <sheet name="CreateMaleEmployee" r:id="rId3" sheetId="14"/>
+    <sheet name="UpdateTaxCodeAndAnnualSalary" r:id="rId4" sheetId="15"/>
+    <sheet name="ProcessPayrolFor20FourWeeklySSP" r:id="rId5" sheetId="1"/>
+    <sheet name="ProcessPayrolFor24FourWeeklySSP" r:id="rId6" sheetId="3"/>
+    <sheet name="ProcessPayrolFor28FourWeeklySSP" r:id="rId7" sheetId="4"/>
+    <sheet name="CreateLeaveRequest" r:id="rId8" sheetId="9"/>
+    <sheet name="UpdateLeaveRecord" r:id="rId9" sheetId="10"/>
+    <sheet name="AverageWeeklyEarningsTestReport" r:id="rId10" sheetId="19"/>
+    <sheet name="ProcessPayrolFor32FourWeeklySSP" r:id="rId11" sheetId="6"/>
+    <sheet name="ProcessPayrolFor36FourWeeklySSP" r:id="rId12" sheetId="7"/>
+    <sheet name="CreateLeaveRequest2" r:id="rId13" sheetId="11"/>
+    <sheet name="UpdateLeaveRecord2" r:id="rId14" sheetId="12"/>
+    <sheet name="AverageWeeklyEarningsTestReprt2" r:id="rId15" sheetId="22"/>
+    <sheet name="ProcessPayrolFor40FourWeeklySSP" r:id="rId16" sheetId="8"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="190">
   <si>
     <t>EmpName</t>
   </si>
@@ -605,6 +605,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,65 +677,65 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="2"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -748,10 +749,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -909,7 +910,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -918,13 +919,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -934,7 +935,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -943,7 +944,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -952,7 +953,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -962,12 +963,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -998,7 +999,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1017,7 +1018,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1029,7 +1030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1038,11 +1039,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27" r="2" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>174</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="22.8" r="3" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="24.6" r="4" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>170</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="31.2" r="5" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>172</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="25.8" r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="7" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="9" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="10" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1182,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="11" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="12" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="13" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="14" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="16" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="18" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="19" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="20" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="21" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>176</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="22" s="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1365,13 +1366,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1380,20 +1381,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1477,16 +1478,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1495,20 +1496,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1592,15 +1593,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1609,21 +1610,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1707,15 +1708,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1724,16 +1725,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="33.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1786,12 +1787,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1800,15 +1801,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1861,12 +1862,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1875,21 +1876,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="43.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="43.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1973,15 +1974,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
@@ -1990,21 +1991,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2088,15 +2089,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2105,13 +2106,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2152,12 +2153,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2166,17 +2167,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -2554,15 +2555,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2571,15 +2572,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2626,12 +2627,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2640,19 +2641,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2736,15 +2737,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2753,19 +2754,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="44.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2849,15 +2850,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2866,21 +2867,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="39" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="20" customFormat="1" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2964,15 +2965,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000005uTn1" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2981,16 +2982,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3049,12 +3050,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3063,16 +3064,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3131,6 +3132,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
optimised Reset script for SSP and ShPP Scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite Statutory SSP201718.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="14" firstSheet="12" windowHeight="5400" windowWidth="15168" xWindow="384" yWindow="36"/>
+    <workbookView activeTab="15" firstSheet="13" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="2"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="191">
   <si>
     <t>EmpName</t>
   </si>
@@ -599,12 +604,15 @@
   </si>
   <si>
     <t>11 December 2017</t>
+  </si>
+  <si>
+    <t>Four Week-28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -748,6 +756,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -795,7 +806,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -828,9 +839,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -863,6 +891,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1045,16 +1090,16 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.28515625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1068,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27" r="2" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27" r="2" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -1082,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="22.8" r="3" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="22.9" r="3" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -1096,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="24.6" r="4" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="24.6" r="4" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>168</v>
       </c>
@@ -1107,7 +1152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="31.2" r="5" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="31.15" r="5" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>170</v>
       </c>
@@ -1121,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="25.8" r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="25.9" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1135,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="7" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="9" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1177,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="10" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="10" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1191,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="11" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1205,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="12" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="12" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="13" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1233,7 +1278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="14" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="14" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1247,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1261,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="16" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1275,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1289,7 +1334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="18" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1303,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="19" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1317,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="20" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="20" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1331,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="21" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>174</v>
       </c>
@@ -1345,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="22" s="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="22" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1359,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1387,22 +1432,22 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="39.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="39.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="39.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1446,7 +1491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1501,22 +1546,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="32.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="37.6640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1560,7 +1605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1614,23 +1659,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1674,7 +1719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1728,18 +1773,18 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="33.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="33.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1804,17 +1849,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="36.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +1888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1876,27 +1921,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="37.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="43.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.21875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -1940,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -1990,27 +2035,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.85546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2054,7 +2099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2108,15 +2153,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2169,19 +2214,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:63" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
@@ -2372,7 +2417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:63" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -2574,17 +2619,17 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2610,7 +2655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="21.6" r="2" s="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2643,21 +2688,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="42.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2701,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2756,21 +2801,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.21875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="44.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2814,7 +2859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2865,26 +2910,26 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.140625" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -2928,7 +2973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.8" r="2" s="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>187</v>
       </c>
@@ -2942,7 +2987,7 @@
         <v>133</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>151</v>
@@ -2982,18 +3027,18 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.7109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3025,7 +3070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3064,18 +3109,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="34.21875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3107,7 +3152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>